<commit_message>
Fix met file address and graphinc at Narrabri23
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/Narrabri23.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/Narrabri23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E43ABAC-A647-41BC-9077-9F1ECA72AAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8BAF88-7D50-4F37-8149-3225988EC708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -500,12 +500,6 @@
     <t>dw_Bur</t>
   </si>
   <si>
-    <t>Bur.NConc</t>
-  </si>
-  <si>
-    <t>Bur.N</t>
-  </si>
-  <si>
     <t>Cotton.Seed.N</t>
   </si>
   <si>
@@ -582,6 +576,12 @@
   </si>
   <si>
     <t>Soil.Water.Volumetric(9)</t>
+  </si>
+  <si>
+    <t>Cotton.Bur.NConc</t>
+  </si>
+  <si>
+    <t>Cotton.Bur.N</t>
   </si>
 </sst>
 </file>
@@ -991,10 +991,10 @@
   <dimension ref="A1:FJ293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="DJ54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="BH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DK90" sqref="DK90"/>
+      <selection pane="bottomRight" activeCell="BS1" sqref="BS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1314,10 +1314,10 @@
         <v>153</v>
       </c>
       <c r="BC1" s="12" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="BD1" s="12" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="BE1" t="s">
         <v>102</v>
@@ -1347,7 +1347,7 @@
         <v>107</v>
       </c>
       <c r="BN1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="BO1" t="s">
         <v>9</v>
@@ -1359,10 +1359,10 @@
         <v>127</v>
       </c>
       <c r="BR1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="BS1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="BT1" t="s">
         <v>108</v>
@@ -1428,7 +1428,7 @@
         <v>67</v>
       </c>
       <c r="CO1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="CP1" t="s">
         <v>89</v>
@@ -1437,88 +1437,88 @@
         <v>113</v>
       </c>
       <c r="CR1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CS1" t="s">
         <v>76</v>
       </c>
       <c r="CT1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="CU1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="CV1" t="s">
         <v>77</v>
       </c>
       <c r="CW1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="CX1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="CY1" t="s">
         <v>85</v>
       </c>
       <c r="CZ1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="DA1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="DB1" t="s">
         <v>84</v>
       </c>
       <c r="DC1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="DD1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DE1" t="s">
         <v>83</v>
       </c>
       <c r="DF1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="DG1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DH1" t="s">
         <v>94</v>
       </c>
       <c r="DI1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="DJ1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="DK1" t="s">
         <v>95</v>
       </c>
       <c r="DL1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="DM1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DN1" t="s">
         <v>82</v>
       </c>
       <c r="DO1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="DP1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="DQ1" t="s">
         <v>81</v>
       </c>
       <c r="DR1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="DS1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="DT1" t="s">
         <v>80</v>
@@ -1527,7 +1527,7 @@
         <v>86</v>
       </c>
       <c r="DV1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="DW1" t="s">
         <v>79</v>
@@ -1536,7 +1536,7 @@
         <v>87</v>
       </c>
       <c r="DY1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="DZ1" t="s">
         <v>78</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="2" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="3" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="4" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="5" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="6" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="7" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2135,7 +2135,7 @@
     </row>
     <row r="8" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="9" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="10" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="11" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="12" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="13" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="14" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="15" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2874,7 +2874,7 @@
     </row>
     <row r="16" spans="1:166" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="17" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="18" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="19" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="20" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="21" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="22" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="23" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="24" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="25" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="26" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="27" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3982,7 +3982,7 @@
     </row>
     <row r="28" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4029,7 +4029,7 @@
     </row>
     <row r="29" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4131,7 +4131,7 @@
     </row>
     <row r="30" spans="1:122" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B30">
         <v>1</v>

</xml_diff>

<commit_message>
Improve height and node number models
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/Narrabri23.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/Narrabri23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8BAF88-7D50-4F37-8149-3225988EC708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E245B915-BEE6-4459-815F-A4FB842506BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -994,7 +994,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="BH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BS1" sqref="BS1"/>
+      <selection pane="bottomRight" activeCell="BS2" sqref="BS2:BS87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4186,7 +4186,6 @@
         <v>3.0167499999999996E-2</v>
       </c>
       <c r="BS30" s="3">
-        <f>BQ30*BR30</f>
         <v>7.5607315438885241</v>
       </c>
       <c r="BT30" s="3">
@@ -6734,7 +6733,6 @@
         <v>3.2247500000000005E-2</v>
       </c>
       <c r="BS59" s="3">
-        <f>BQ59*BR59</f>
         <v>9.1988246605529689</v>
       </c>
       <c r="BT59" s="3">
@@ -9252,7 +9250,6 @@
         <v>3.6049999999999999E-2</v>
       </c>
       <c r="BS87" s="3">
-        <f>BQ87*BR87</f>
         <v>12.276870777924218</v>
       </c>
       <c r="BT87" s="3">

</xml_diff>